<commit_message>
added pivot tables for LEAD categories
</commit_message>
<xml_diff>
--- a/SalesForceByMonth1.xlsx
+++ b/SalesForceByMonth1.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjc341\Desktop\EMSA-GIT\COLAB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="PRIOR" sheetId="2" r:id="rId2"/>
+    <sheet name="LEAD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>MONTH</t>
   </si>
@@ -72,16 +78,76 @@
   </si>
   <si>
     <t>Prior to Jan 2018</t>
+  </si>
+  <si>
+    <t>Lead_Source</t>
+  </si>
+  <si>
+    <t>College Fair</t>
+  </si>
+  <si>
+    <t>College Visit</t>
+  </si>
+  <si>
+    <t>Education Fair</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Event Registration</t>
+  </si>
+  <si>
+    <t>Group Tour</t>
+  </si>
+  <si>
+    <t>High School Visit</t>
+  </si>
+  <si>
+    <t>Initiated Application</t>
+  </si>
+  <si>
+    <t>International Travel</t>
+  </si>
+  <si>
+    <t>Lead Card</t>
+  </si>
+  <si>
+    <t>Office Visit</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Professional Conference</t>
+  </si>
+  <si>
+    <t>Purchased List</t>
+  </si>
+  <si>
+    <t>Submitted Test Score</t>
+  </si>
+  <si>
+    <t>UGrad Campus Visit Check-in Form</t>
+  </si>
+  <si>
+    <t>Virtual Tour</t>
+  </si>
+  <si>
+    <t>Web Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##,###"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +224,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +278,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,9 +310,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,6 +345,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,18 +521,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -487,7 +563,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -504,7 +580,7 @@
         <v>2754</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -521,7 +597,7 @@
         <v>9018</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -538,7 +614,7 @@
         <v>11967</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -555,7 +631,7 @@
         <v>7052</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -572,7 +648,7 @@
         <v>11067</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1">
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -589,7 +665,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -606,7 +682,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1">
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -623,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1">
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -640,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1">
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -657,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1">
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -680,18 +756,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -702,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -716,7 +792,307 @@
         <v>27464</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1"/>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>7783</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5208</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5604</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>116</v>
+      </c>
+      <c r="C5" s="3">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8074</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9131</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3">
+        <v>252</v>
+      </c>
+      <c r="C7" s="3">
+        <v>279</v>
+      </c>
+      <c r="D7" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5427</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5410</v>
+      </c>
+      <c r="D8" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3">
+        <v>9010</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3">
+        <v>148</v>
+      </c>
+      <c r="C11" s="3">
+        <v>175</v>
+      </c>
+      <c r="D11" s="3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3">
+        <v>200</v>
+      </c>
+      <c r="C12" s="3">
+        <v>131</v>
+      </c>
+      <c r="D12" s="3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1208</v>
+      </c>
+      <c r="C13" s="3">
+        <v>352</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3">
+        <v>13154</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16100</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10613</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3">
+        <v>48580</v>
+      </c>
+      <c r="C17" s="3">
+        <v>43434</v>
+      </c>
+      <c r="D17" s="3">
+        <v>15815</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3">
+        <v>115</v>
+      </c>
+      <c r="C19" s="3">
+        <v>812</v>
+      </c>
+      <c r="D19" s="3">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3">
+        <v>6605</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5380</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the col names
</commit_message>
<xml_diff>
--- a/SalesForceByMonth1.xlsx
+++ b/SalesForceByMonth1.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjc341\Desktop\EMSA-GIT\COLAB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="PRIOR" sheetId="2" r:id="rId2"/>
     <sheet name="LEAD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>MONTH</t>
   </si>
@@ -78,6 +73,15 @@
   </si>
   <si>
     <t>Prior to Jan 2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
   </si>
   <si>
     <t>Lead_Source</t>
@@ -143,11 +147,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##,###"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,14 +228,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -278,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -310,10 +306,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,7 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,18 +515,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -563,7 +557,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -580,7 +574,7 @@
         <v>2754</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="2" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -597,7 +591,7 @@
         <v>9018</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="2" customFormat="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -614,7 +608,7 @@
         <v>11967</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="2" customFormat="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -631,7 +625,7 @@
         <v>7052</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="2" customFormat="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -648,7 +642,7 @@
         <v>11067</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="2" customFormat="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -665,7 +659,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="2" customFormat="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -682,7 +676,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="2" customFormat="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -699,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="2" customFormat="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -716,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -733,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="2" customFormat="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -756,18 +750,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -778,7 +772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -792,43 +786,41 @@
         <v>27464</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" s="3" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3">
         <v>7783</v>
@@ -840,9 +832,9 @@
         <v>5604</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="3" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -854,9 +846,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="3" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -868,9 +860,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="3" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>116</v>
@@ -882,9 +874,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="3" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>8074</v>
@@ -896,9 +888,9 @@
         <v>8803</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3">
         <v>252</v>
@@ -910,9 +902,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="3" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <v>5427</v>
@@ -924,9 +916,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="3" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3">
         <v>9010</v>
@@ -938,9 +930,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="3" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -952,9 +944,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="3" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3">
         <v>148</v>
@@ -966,9 +958,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="3" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3">
         <v>200</v>
@@ -980,9 +972,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="3" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>1208</v>
@@ -994,9 +986,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="3" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3">
         <v>17</v>
@@ -1008,9 +1000,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="3" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -1022,9 +1014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="3" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3">
         <v>13154</v>
@@ -1036,9 +1028,9 @@
         <v>10613</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="3" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3">
         <v>48580</v>
@@ -1050,9 +1042,9 @@
         <v>15815</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="3" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -1064,9 +1056,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="3" customFormat="1">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3">
         <v>115</v>
@@ -1078,9 +1070,9 @@
         <v>862</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="3" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B20" s="3">
         <v>6605</v>
@@ -1092,7 +1084,7 @@
         <v>4497</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:4" s="3" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the code from the MERGE branch
</commit_message>
<xml_diff>
--- a/SalesForceByMonth1.xlsx
+++ b/SalesForceByMonth1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjc341\Desktop\EMSA-GIT\COLAB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="PRIOR" sheetId="2" r:id="rId2"/>
     <sheet name="LEAD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -147,11 +152,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##,###"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +233,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -274,7 +287,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,9 +319,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,6 +354,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -515,18 +530,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -548,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>3503</v>
+        <v>3501</v>
       </c>
       <c r="D2" s="2">
         <v>1882</v>
@@ -557,7 +572,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -568,13 +583,13 @@
         <v>4667</v>
       </c>
       <c r="D3" s="2">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="E3" s="2">
         <v>2754</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -585,13 +600,13 @@
         <v>1686</v>
       </c>
       <c r="D4" s="2">
-        <v>3614</v>
+        <v>3612</v>
       </c>
       <c r="E4" s="2">
         <v>9018</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -599,16 +614,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="D5" s="2">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="E5" s="2">
         <v>11967</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -619,13 +634,13 @@
         <v>2547</v>
       </c>
       <c r="D6" s="2">
-        <v>10576</v>
+        <v>10571</v>
       </c>
       <c r="E6" s="2">
         <v>7052</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -633,16 +648,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="2">
-        <v>12483</v>
+        <v>12482</v>
       </c>
       <c r="D7" s="2">
-        <v>6946</v>
+        <v>6944</v>
       </c>
       <c r="E7" s="2">
         <v>11067</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1">
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -650,7 +665,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2">
-        <v>12933</v>
+        <v>12931</v>
       </c>
       <c r="D8" s="2">
         <v>3798</v>
@@ -659,7 +674,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -670,13 +685,13 @@
         <v>2435</v>
       </c>
       <c r="D9" s="2">
-        <v>4993</v>
+        <v>4991</v>
       </c>
       <c r="E9" s="2">
-        <v>2471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -684,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2">
-        <v>7714</v>
+        <v>7711</v>
       </c>
       <c r="D10" s="2">
         <v>5989</v>
@@ -693,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1">
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -701,16 +716,16 @@
         <v>13</v>
       </c>
       <c r="C11" s="2">
-        <v>18403</v>
+        <v>18401</v>
       </c>
       <c r="D11" s="2">
-        <v>20881</v>
+        <v>20878</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1">
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -718,7 +733,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="2">
-        <v>17757</v>
+        <v>17755</v>
       </c>
       <c r="D12" s="2">
         <v>15739</v>
@@ -727,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1">
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -750,18 +765,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -772,39 +787,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>58727</v>
+        <v>58709</v>
       </c>
       <c r="C2" s="3">
-        <v>35764</v>
+        <v>35755</v>
       </c>
       <c r="D2" s="3">
-        <v>27464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1"/>
+        <v>27462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -818,21 +833,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="3">
-        <v>7783</v>
+        <v>7782</v>
       </c>
       <c r="C2" s="3">
-        <v>5208</v>
+        <v>5205</v>
       </c>
       <c r="D2" s="3">
         <v>5604</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -846,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1">
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -860,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1">
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -874,21 +889,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="3">
-        <v>8074</v>
+        <v>8072</v>
       </c>
       <c r="C6" s="3">
-        <v>9131</v>
+        <v>9130</v>
       </c>
       <c r="D6" s="3">
-        <v>8803</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1">
+        <v>8606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -896,13 +911,13 @@
         <v>252</v>
       </c>
       <c r="C7" s="3">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D7" s="3">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1">
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -916,7 +931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1">
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -930,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -944,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1">
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -958,7 +973,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1">
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -969,10 +984,10 @@
         <v>131</v>
       </c>
       <c r="D12" s="3">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="3" customFormat="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -983,10 +998,10 @@
         <v>352</v>
       </c>
       <c r="D13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="3" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1000,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1">
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1014,35 +1029,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="3">
-        <v>13154</v>
+        <v>13153</v>
       </c>
       <c r="C16" s="3">
-        <v>16100</v>
+        <v>16096</v>
       </c>
       <c r="D16" s="3">
         <v>10613</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1">
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="3">
-        <v>48580</v>
+        <v>48571</v>
       </c>
       <c r="C17" s="3">
-        <v>43434</v>
+        <v>43428</v>
       </c>
       <c r="D17" s="3">
-        <v>15815</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="3" customFormat="1">
+        <v>15606</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1">
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1064,13 +1079,13 @@
         <v>115</v>
       </c>
       <c r="C19" s="3">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D19" s="3">
         <v>862</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1081,10 +1096,10 @@
         <v>5380</v>
       </c>
       <c r="D20" s="3">
-        <v>4497</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="3" customFormat="1"/>
+        <v>4319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
COmpleted the states code
</commit_message>
<xml_diff>
--- a/SalesForceByMonth1.xlsx
+++ b/SalesForceByMonth1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="TOTAL4" sheetId="5" r:id="rId5"/>
     <sheet name="LEAD" sheetId="6" r:id="rId6"/>
     <sheet name="ETH2" sheetId="7" r:id="rId7"/>
+    <sheet name="ST2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
   <si>
     <t>MONTH</t>
   </si>
@@ -220,6 +221,177 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>STATE5</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WY</t>
   </si>
 </sst>
 </file>
@@ -606,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1423,7 +1595,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1557,4 +1729,817 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1812</v>
+      </c>
+      <c r="C3" s="3">
+        <v>698</v>
+      </c>
+      <c r="D3" s="3">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3">
+        <v>454</v>
+      </c>
+      <c r="C4" s="3">
+        <v>256</v>
+      </c>
+      <c r="D4" s="3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3">
+        <v>781</v>
+      </c>
+      <c r="C5" s="3">
+        <v>452</v>
+      </c>
+      <c r="D5" s="3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4642</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3278</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="3">
+        <v>858</v>
+      </c>
+      <c r="C7" s="3">
+        <v>722</v>
+      </c>
+      <c r="D7" s="3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1282</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1219</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3">
+        <v>129</v>
+      </c>
+      <c r="D9" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="3">
+        <v>290</v>
+      </c>
+      <c r="C10" s="3">
+        <v>246</v>
+      </c>
+      <c r="D10" s="3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3">
+        <v>31935</v>
+      </c>
+      <c r="C11" s="3">
+        <v>26867</v>
+      </c>
+      <c r="D11" s="3">
+        <v>26372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3528</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2541</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3">
+        <v>382</v>
+      </c>
+      <c r="C15" s="3">
+        <v>300</v>
+      </c>
+      <c r="D15" s="3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="3">
+        <v>254</v>
+      </c>
+      <c r="C16" s="3">
+        <v>117</v>
+      </c>
+      <c r="D16" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3">
+        <v>143</v>
+      </c>
+      <c r="C17" s="3">
+        <v>38</v>
+      </c>
+      <c r="D17" s="3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3901</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3261</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1183</v>
+      </c>
+      <c r="C19" s="3">
+        <v>538</v>
+      </c>
+      <c r="D19" s="3">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3">
+        <v>331</v>
+      </c>
+      <c r="C20" s="3">
+        <v>195</v>
+      </c>
+      <c r="D20" s="3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1169</v>
+      </c>
+      <c r="C21" s="3">
+        <v>468</v>
+      </c>
+      <c r="D21" s="3">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1334</v>
+      </c>
+      <c r="C22" s="3">
+        <v>721</v>
+      </c>
+      <c r="D22" s="3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2037</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1687</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2551</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1970</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="3">
+        <v>133</v>
+      </c>
+      <c r="C25" s="3">
+        <v>77</v>
+      </c>
+      <c r="D25" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1311</v>
+      </c>
+      <c r="C27" s="3">
+        <v>908</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1319</v>
+      </c>
+      <c r="C28" s="3">
+        <v>667</v>
+      </c>
+      <c r="D28" s="3">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="3">
+        <v>948</v>
+      </c>
+      <c r="C29" s="3">
+        <v>596</v>
+      </c>
+      <c r="D29" s="3">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="3">
+        <v>309</v>
+      </c>
+      <c r="C30" s="3">
+        <v>251</v>
+      </c>
+      <c r="D30" s="3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="3">
+        <v>64</v>
+      </c>
+      <c r="C31" s="3">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="3">
+        <v>4888</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1664</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="3">
+        <v>36</v>
+      </c>
+      <c r="C33" s="3">
+        <v>26</v>
+      </c>
+      <c r="D33" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="3">
+        <v>238</v>
+      </c>
+      <c r="C34" s="3">
+        <v>170</v>
+      </c>
+      <c r="D34" s="3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="3">
+        <v>248</v>
+      </c>
+      <c r="C35" s="3">
+        <v>195</v>
+      </c>
+      <c r="D35" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4738</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4322</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="3">
+        <v>201</v>
+      </c>
+      <c r="C37" s="3">
+        <v>54</v>
+      </c>
+      <c r="D37" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="3">
+        <v>333</v>
+      </c>
+      <c r="C38" s="3">
+        <v>139</v>
+      </c>
+      <c r="D38" s="3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="3">
+        <v>5161</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4637</v>
+      </c>
+      <c r="D39" s="3">
+        <v>5463</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2412</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D40" s="3">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="3">
+        <v>755</v>
+      </c>
+      <c r="C41" s="3">
+        <v>234</v>
+      </c>
+      <c r="D41" s="3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="3">
+        <v>283</v>
+      </c>
+      <c r="C42" s="3">
+        <v>120</v>
+      </c>
+      <c r="D42" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="3">
+        <v>3230</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2441</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="3">
+        <v>160</v>
+      </c>
+      <c r="C44" s="3">
+        <v>204</v>
+      </c>
+      <c r="D44" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="3">
+        <v>255</v>
+      </c>
+      <c r="C45" s="3">
+        <v>231</v>
+      </c>
+      <c r="D45" s="3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1171</v>
+      </c>
+      <c r="C46" s="3">
+        <v>733</v>
+      </c>
+      <c r="D46" s="3">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45</v>
+      </c>
+      <c r="C47" s="3">
+        <v>23</v>
+      </c>
+      <c r="D47" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="3">
+        <v>3045</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1252</v>
+      </c>
+      <c r="D48" s="3">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="3">
+        <v>5191</v>
+      </c>
+      <c r="C49" s="3">
+        <v>3656</v>
+      </c>
+      <c r="D49" s="3">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="3">
+        <v>754</v>
+      </c>
+      <c r="C50" s="3">
+        <v>167</v>
+      </c>
+      <c r="D50" s="3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2014</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1326</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="3">
+        <v>37</v>
+      </c>
+      <c r="C52" s="3">
+        <v>12</v>
+      </c>
+      <c r="D52" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="3">
+        <v>96</v>
+      </c>
+      <c r="C53" s="3">
+        <v>77</v>
+      </c>
+      <c r="D53" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="3">
+        <v>670</v>
+      </c>
+      <c r="C54" s="3">
+        <v>295</v>
+      </c>
+      <c r="D54" s="3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="3">
+        <v>716</v>
+      </c>
+      <c r="C55" s="3">
+        <v>452</v>
+      </c>
+      <c r="D55" s="3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="3">
+        <v>223</v>
+      </c>
+      <c r="C56" s="3">
+        <v>66</v>
+      </c>
+      <c r="D56" s="3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="3">
+        <v>34</v>
+      </c>
+      <c r="C57" s="3">
+        <v>26</v>
+      </c>
+      <c r="D57" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>